<commit_message>
Fix missing dictionary attributes
Fixed some missing dictionary attributes with # of seniors and workplace address for census profile.
</commit_message>
<xml_diff>
--- a/data/PQ data/Dictionaries/PQCHC_data_plan_dictionary.xlsx
+++ b/data/PQ data/Dictionaries/PQCHC_data_plan_dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4617e70f33205b2a/Documents/GitHub/2021_CensusDataProcessing/data/PQ data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ANZO NGUYEN\Pictures\Documents\GitHub\2021_CensusDataProcessing\data\PQ data\Dictionaries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="887" documentId="8_{CE446891-56C3-46A0-B41E-B43D6D107E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2A209FC1-7C0A-42EF-B718-DAC0071B261B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C423041-17C1-414D-BC6D-E2173D56CB7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" firstSheet="1" activeTab="2" xr2:uid="{78EF0FB6-9AB1-4EDB-B7C7-CDF5A0E6492F}"/>
+    <workbookView xWindow="15120" yWindow="135" windowWidth="13605" windowHeight="15465" firstSheet="1" activeTab="2" xr2:uid="{78EF0FB6-9AB1-4EDB-B7C7-CDF5A0E6492F}"/>
   </bookViews>
   <sheets>
     <sheet name="Selected Data IDs" sheetId="1" r:id="rId1"/>
@@ -1730,18 +1730,18 @@
       <selection activeCell="A29" sqref="A29:B29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.73046875" customWidth="1"/>
-    <col min="7" max="7" width="20.59765625" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" customWidth="1"/>
     <col min="8" max="8" width="60" customWidth="1"/>
-    <col min="9" max="9" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1749,7 +1749,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -1773,7 +1773,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -1781,7 +1781,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -1789,7 +1789,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
@@ -1797,7 +1797,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -1805,7 +1805,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
@@ -1813,7 +1813,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -1821,7 +1821,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>20</v>
       </c>
@@ -1829,7 +1829,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1837,7 +1837,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>24</v>
       </c>
@@ -1845,7 +1845,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>26</v>
       </c>
@@ -1853,7 +1853,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -1861,7 +1861,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>30</v>
       </c>
@@ -1869,7 +1869,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>32</v>
       </c>
@@ -1877,7 +1877,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>34</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1893,7 +1893,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>38</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>40</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -1917,7 +1917,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>44</v>
       </c>
@@ -1925,7 +1925,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
@@ -1933,7 +1933,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>48</v>
       </c>
@@ -1941,11 +1941,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -1953,7 +1953,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>52</v>
       </c>
@@ -1961,7 +1961,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>54</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>56</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>58</v>
       </c>
@@ -1985,7 +1985,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>60</v>
       </c>
@@ -1993,7 +1993,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>62</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>64</v>
       </c>
@@ -2009,7 +2009,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>66</v>
       </c>
@@ -2017,7 +2017,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>68</v>
       </c>
@@ -2025,7 +2025,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>70</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>72</v>
       </c>
@@ -2041,7 +2041,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -2049,7 +2049,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>76</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>78</v>
       </c>
@@ -2065,7 +2065,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>80</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>82</v>
       </c>
@@ -2081,7 +2081,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>84</v>
       </c>
@@ -2089,7 +2089,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -2105,7 +2105,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>90</v>
       </c>
@@ -2113,7 +2113,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>92</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>94</v>
       </c>
@@ -2129,7 +2129,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>96</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>98</v>
       </c>
@@ -2145,7 +2145,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>100</v>
       </c>
@@ -2153,7 +2153,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>102</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>104</v>
       </c>
@@ -2169,7 +2169,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>106</v>
       </c>
@@ -2177,7 +2177,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>108</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>110</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>112</v>
       </c>
@@ -2201,7 +2201,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>114</v>
       </c>
@@ -2209,7 +2209,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>116</v>
       </c>
@@ -2217,7 +2217,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>118</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>120</v>
       </c>
@@ -2233,7 +2233,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>122</v>
       </c>
@@ -2241,7 +2241,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>124</v>
       </c>
@@ -2249,7 +2249,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>126</v>
       </c>
@@ -2257,7 +2257,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>128</v>
       </c>
@@ -2265,7 +2265,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>130</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>132</v>
       </c>
@@ -2281,7 +2281,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>134</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>136</v>
       </c>
@@ -2297,7 +2297,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>138</v>
       </c>
@@ -2305,7 +2305,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>140</v>
       </c>
@@ -2313,7 +2313,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>142</v>
       </c>
@@ -2321,7 +2321,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>144</v>
       </c>
@@ -2329,7 +2329,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>146</v>
       </c>
@@ -2337,7 +2337,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
         <v>148</v>
       </c>
@@ -2345,7 +2345,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>150</v>
       </c>
@@ -2353,7 +2353,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
         <v>152</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>154</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
         <v>156</v>
       </c>
@@ -2377,7 +2377,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
         <v>158</v>
       </c>
@@ -2385,7 +2385,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
         <v>160</v>
       </c>
@@ -2393,7 +2393,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>162</v>
       </c>
@@ -2401,7 +2401,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>164</v>
       </c>
@@ -2409,7 +2409,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>166</v>
       </c>
@@ -2417,7 +2417,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>168</v>
       </c>
@@ -2425,7 +2425,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
         <v>170</v>
       </c>
@@ -2433,7 +2433,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>172</v>
       </c>
@@ -2441,7 +2441,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>174</v>
       </c>
@@ -2449,7 +2449,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>176</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
         <v>178</v>
       </c>
@@ -2465,7 +2465,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
         <v>180</v>
       </c>
@@ -2473,7 +2473,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
         <v>182</v>
       </c>
@@ -2481,7 +2481,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
         <v>184</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>186</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>188</v>
       </c>
@@ -2505,7 +2505,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
         <v>190</v>
       </c>
@@ -2513,7 +2513,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
         <v>192</v>
       </c>
@@ -2521,7 +2521,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
         <v>194</v>
       </c>
@@ -2529,7 +2529,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>196</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>198</v>
       </c>
@@ -2545,7 +2545,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>200</v>
       </c>
@@ -2553,7 +2553,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>202</v>
       </c>
@@ -2561,7 +2561,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
         <v>204</v>
       </c>
@@ -2569,7 +2569,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>206</v>
       </c>
@@ -2577,7 +2577,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>208</v>
       </c>
@@ -2585,7 +2585,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>210</v>
       </c>
@@ -2593,7 +2593,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>212</v>
       </c>
@@ -2601,7 +2601,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>214</v>
       </c>
@@ -2609,7 +2609,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>216</v>
       </c>
@@ -2617,7 +2617,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>218</v>
       </c>
@@ -2625,7 +2625,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>220</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>222</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>224</v>
       </c>
@@ -2649,7 +2649,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>226</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>228</v>
       </c>
@@ -2665,7 +2665,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>230</v>
       </c>
@@ -2673,7 +2673,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>232</v>
       </c>
@@ -2681,7 +2681,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>233</v>
       </c>
@@ -2689,7 +2689,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>234</v>
       </c>
@@ -2697,7 +2697,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>235</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>236</v>
       </c>
@@ -2713,7 +2713,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>237</v>
       </c>
@@ -2721,7 +2721,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>238</v>
       </c>
@@ -2729,7 +2729,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>239</v>
       </c>
@@ -2737,7 +2737,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>240</v>
       </c>
@@ -2745,7 +2745,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>242</v>
       </c>
@@ -2753,7 +2753,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>244</v>
       </c>
@@ -2761,7 +2761,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>246</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>248</v>
       </c>
@@ -2777,7 +2777,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>250</v>
       </c>
@@ -2785,7 +2785,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>252</v>
       </c>
@@ -2793,7 +2793,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>253</v>
       </c>
@@ -2801,7 +2801,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>254</v>
       </c>
@@ -2809,7 +2809,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>256</v>
       </c>
@@ -2817,7 +2817,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>258</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
         <v>260</v>
       </c>
@@ -2833,7 +2833,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>262</v>
       </c>
@@ -2841,7 +2841,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>264</v>
       </c>
@@ -2849,7 +2849,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>266</v>
       </c>
@@ -2857,7 +2857,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>268</v>
       </c>
@@ -2865,7 +2865,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>270</v>
       </c>
@@ -2873,7 +2873,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>272</v>
       </c>
@@ -2881,7 +2881,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>274</v>
       </c>
@@ -2889,7 +2889,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>276</v>
       </c>
@@ -2913,16 +2913,16 @@
       <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="63.265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="63.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>278</v>
       </c>
@@ -2939,7 +2939,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -2956,7 +2956,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>286</v>
       </c>
@@ -2973,7 +2973,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>288</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>290</v>
       </c>
@@ -3007,7 +3007,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>291</v>
       </c>
@@ -3024,7 +3024,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>294</v>
       </c>
@@ -3041,7 +3041,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>295</v>
       </c>
@@ -3058,7 +3058,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>297</v>
       </c>
@@ -3075,7 +3075,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>298</v>
       </c>
@@ -3092,7 +3092,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>299</v>
       </c>
@@ -3109,7 +3109,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>300</v>
       </c>
@@ -3126,7 +3126,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>301</v>
       </c>
@@ -3143,7 +3143,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>302</v>
       </c>
@@ -3160,7 +3160,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>303</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>305</v>
       </c>
@@ -3194,7 +3194,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>307</v>
       </c>
@@ -3211,7 +3211,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>309</v>
       </c>
@@ -3228,7 +3228,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>311</v>
       </c>
@@ -3245,7 +3245,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -3262,7 +3262,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>313</v>
       </c>
@@ -3279,7 +3279,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>314</v>
       </c>
@@ -3296,7 +3296,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>315</v>
       </c>
@@ -3313,7 +3313,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>316</v>
       </c>
@@ -3330,7 +3330,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>317</v>
       </c>
@@ -3347,7 +3347,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>318</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>319</v>
       </c>
@@ -3381,7 +3381,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>320</v>
       </c>
@@ -3398,7 +3398,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>321</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>322</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>323</v>
       </c>
@@ -3449,7 +3449,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>324</v>
       </c>
@@ -3466,7 +3466,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>325</v>
       </c>
@@ -3483,7 +3483,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>326</v>
       </c>
@@ -3500,7 +3500,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>327</v>
       </c>
@@ -3517,7 +3517,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>328</v>
       </c>
@@ -3534,7 +3534,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>329</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>330</v>
       </c>
@@ -3568,7 +3568,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>331</v>
       </c>
@@ -3585,7 +3585,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>332</v>
       </c>
@@ -3602,7 +3602,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>333</v>
       </c>
@@ -3619,7 +3619,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>334</v>
       </c>
@@ -3636,7 +3636,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>335</v>
       </c>
@@ -3653,7 +3653,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>336</v>
       </c>
@@ -3670,7 +3670,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>337</v>
       </c>
@@ -3687,7 +3687,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>338</v>
       </c>
@@ -3704,7 +3704,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>339</v>
       </c>
@@ -3721,7 +3721,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>340</v>
       </c>
@@ -3738,7 +3738,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>341</v>
       </c>
@@ -3755,7 +3755,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>342</v>
       </c>
@@ -3772,7 +3772,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>343</v>
       </c>
@@ -3789,7 +3789,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>344</v>
       </c>
@@ -3806,7 +3806,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>345</v>
       </c>
@@ -3823,7 +3823,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>346</v>
       </c>
@@ -3840,7 +3840,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>347</v>
       </c>
@@ -3857,7 +3857,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>348</v>
       </c>
@@ -3874,7 +3874,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>349</v>
       </c>
@@ -3891,7 +3891,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>350</v>
       </c>
@@ -3908,7 +3908,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>351</v>
       </c>
@@ -3925,7 +3925,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>149</v>
       </c>
@@ -3942,7 +3942,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>261</v>
       </c>
@@ -3959,7 +3959,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>352</v>
       </c>
@@ -3976,7 +3976,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>353</v>
       </c>
@@ -3993,7 +3993,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>355</v>
       </c>
@@ -4010,7 +4010,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>356</v>
       </c>
@@ -4027,7 +4027,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>357</v>
       </c>
@@ -4044,7 +4044,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>358</v>
       </c>
@@ -4061,7 +4061,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>359</v>
       </c>
@@ -4078,7 +4078,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>361</v>
       </c>
@@ -4095,7 +4095,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>362</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>363</v>
       </c>
@@ -4129,7 +4129,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>364</v>
       </c>
@@ -4146,7 +4146,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>365</v>
       </c>
@@ -4163,7 +4163,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>366</v>
       </c>
@@ -4180,7 +4180,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>367</v>
       </c>
@@ -4197,7 +4197,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>368</v>
       </c>
@@ -4214,7 +4214,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>369</v>
       </c>
@@ -4231,7 +4231,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>370</v>
       </c>
@@ -4248,7 +4248,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>371</v>
       </c>
@@ -4262,7 +4262,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>372</v>
       </c>
@@ -4279,7 +4279,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>373</v>
       </c>
@@ -4293,7 +4293,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>374</v>
       </c>
@@ -4310,7 +4310,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>375</v>
       </c>
@@ -4327,7 +4327,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>376</v>
       </c>
@@ -4344,7 +4344,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>377</v>
       </c>
@@ -4361,7 +4361,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>378</v>
       </c>
@@ -4378,7 +4378,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>379</v>
       </c>
@@ -4395,7 +4395,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>380</v>
       </c>
@@ -4423,19 +4423,19 @@
   <dimension ref="A1:E42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="56.73046875" customWidth="1"/>
-    <col min="2" max="2" width="18.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="56.7109375" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>396</v>
       </c>
@@ -4452,7 +4452,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>392</v>
       </c>
@@ -4469,7 +4469,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>393</v>
       </c>
@@ -4486,7 +4486,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>341</v>
       </c>
@@ -4503,7 +4503,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>342</v>
       </c>
@@ -4520,7 +4520,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>383</v>
       </c>
@@ -4537,7 +4537,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>384</v>
       </c>
@@ -4554,7 +4554,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>381</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>313</v>
       </c>
@@ -4588,7 +4588,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>382</v>
       </c>
@@ -4605,7 +4605,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>314</v>
       </c>
@@ -4622,7 +4622,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>318</v>
       </c>
@@ -4639,7 +4639,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>315</v>
       </c>
@@ -4656,7 +4656,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>316</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>317</v>
       </c>
@@ -4690,7 +4690,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>327</v>
       </c>
@@ -4707,7 +4707,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>328</v>
       </c>
@@ -4724,7 +4724,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>387</v>
       </c>
@@ -4741,7 +4741,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>388</v>
       </c>
@@ -4758,7 +4758,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>295</v>
       </c>
@@ -4775,7 +4775,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>346</v>
       </c>
@@ -4792,7 +4792,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>297</v>
       </c>
@@ -4809,7 +4809,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>347</v>
       </c>
@@ -4826,7 +4826,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>298</v>
       </c>
@@ -4843,7 +4843,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>348</v>
       </c>
@@ -4860,7 +4860,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>299</v>
       </c>
@@ -4877,7 +4877,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>349</v>
       </c>
@@ -4894,7 +4894,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>300</v>
       </c>
@@ -4911,7 +4911,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>380</v>
       </c>
@@ -4928,7 +4928,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -4945,7 +4945,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>385</v>
       </c>
@@ -4962,7 +4962,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>378</v>
       </c>
@@ -4979,7 +4979,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>386</v>
       </c>
@@ -4996,7 +4996,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>370</v>
       </c>
@@ -5013,7 +5013,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>371</v>
       </c>
@@ -5030,7 +5030,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>372</v>
       </c>
@@ -5047,7 +5047,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>373</v>
       </c>
@@ -5064,7 +5064,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>390</v>
       </c>
@@ -5081,7 +5081,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>353</v>
       </c>
@@ -5098,7 +5098,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>355</v>
       </c>
@@ -5115,7 +5115,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>286</v>
       </c>
@@ -5132,7 +5132,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>391</v>
       </c>
@@ -5156,6 +5156,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="fb824588-f366-4339-a49f-7eff4c1b42d9" xsi:nil="true"/>
+    <Lastedited xmlns="124915e9-a20b-402d-bc33-fbef48c2c5dc" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="124915e9-a20b-402d-bc33-fbef48c2c5dc">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006EE7EE696B873A41BEAC8257087746C3" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ef739d34c3db00d072e7fd3175074e46">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="124915e9-a20b-402d-bc33-fbef48c2c5dc" xmlns:ns3="fb824588-f366-4339-a49f-7eff4c1b42d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="757988175f1c3dcec2a34a679bb9ba6b" ns2:_="" ns3:_="">
     <xsd:import namespace="124915e9-a20b-402d-bc33-fbef48c2c5dc"/>
@@ -5404,28 +5425,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E287C00-EF61-4880-92D0-FFAAD3E8160D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="fb824588-f366-4339-a49f-7eff4c1b42d9"/>
+    <ds:schemaRef ds:uri="124915e9-a20b-402d-bc33-fbef48c2c5dc"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="fb824588-f366-4339-a49f-7eff4c1b42d9" xsi:nil="true"/>
-    <Lastedited xmlns="124915e9-a20b-402d-bc33-fbef48c2c5dc" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="124915e9-a20b-402d-bc33-fbef48c2c5dc">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D959687F-11C2-44F9-9F78-B13D5B9F6472}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{26D92BA1-1FBA-4034-8268-15AF08A759B7}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5442,23 +5461,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D959687F-11C2-44F9-9F78-B13D5B9F6472}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E287C00-EF61-4880-92D0-FFAAD3E8160D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="fb824588-f366-4339-a49f-7eff4c1b42d9"/>
-    <ds:schemaRef ds:uri="124915e9-a20b-402d-bc33-fbef48c2c5dc"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>